<commit_message>
dfltServerNum back to 0, now that PSMFC has the latest map services
</commit_message>
<xml_diff>
--- a/Docs/Site Parameters.xlsx
+++ b/Docs/Site Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\ShoreZoneDev_June2024\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFA56C98-A5BB-4E56-8990-F05A414D7F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDC828D-495B-4F70-9C7F-9C4EFA5044C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{154E3D0F-C899-44ED-AAAB-B88943A4BD78}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="14040" xr2:uid="{154E3D0F-C899-44ED-AAAB-B88943A4BD78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve"> When services on the NOAA server are updated but PSMFC hasn't been updated yet, this should be set to 1 for the NOAA server.</t>
   </si>
@@ -91,12 +91,74 @@
       <t>r.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">let </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF830091"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>esriVersion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF830091"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>"4.28"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF080808"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t xml:space="preserve">;     </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Version of the ESRI SDK -- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ESRI puts out a new version 3-4 times each year</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +188,35 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF080808"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF830091"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF830091"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,12 +242,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882D1EDD-D261-4BC8-B0E9-0395E110BABF}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -504,12 +598,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -517,9 +611,17 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="1"/>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>